<commit_message>
carga de archivos para taller 4 y taller 5
</commit_message>
<xml_diff>
--- a/MONITOR/Taller3/Estudiantes.xlsx
+++ b/MONITOR/Taller3/Estudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UJ\UJ2021-01\Monitorias\Taller3\revisionTrabajos\MONITOR\Taller3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\revisionTrabajos\MONITOR\Taller3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B023DAA5-9139-458F-BBC6-065285B70BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9E20EA-9AF5-40DB-9312-7848BE205C0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taller3" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Taller3!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Estudiante</t>
   </si>
@@ -148,6 +151,9 @@
   </si>
   <si>
     <t>Solo había 1 punto, no hay zip</t>
+  </si>
+  <si>
+    <t>Entrega tardía</t>
   </si>
 </sst>
 </file>
@@ -386,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -431,6 +437,7 @@
     <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4352,9 +4359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F23" sqref="F23"/>
+      <selection pane="topRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -4416,6 +4423,14 @@
       <c r="D4" s="6">
         <v>9.6999999999999993</v>
       </c>
+      <c r="G4" s="16">
+        <f>+AVERAGE(B4:D4)</f>
+        <v>9.5333333333333332</v>
+      </c>
+      <c r="H4" s="16">
+        <f>+G4*5/10</f>
+        <v>4.7666666666666666</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
@@ -4430,6 +4445,14 @@
       <c r="D5" s="6">
         <v>10</v>
       </c>
+      <c r="G5" s="16">
+        <f t="shared" ref="G5:G34" si="0">+AVERAGE(B5:D5)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="H5" s="16">
+        <f t="shared" ref="H5:H34" si="1">+G5*5/10</f>
+        <v>4.833333333333333</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -4444,6 +4467,14 @@
       <c r="D6" s="6">
         <v>9.8000000000000007</v>
       </c>
+      <c r="G6" s="16">
+        <f t="shared" si="0"/>
+        <v>9.9333333333333336</v>
+      </c>
+      <c r="H6" s="16">
+        <f t="shared" si="1"/>
+        <v>4.9666666666666668</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="7" t="s">
@@ -4458,6 +4489,14 @@
       <c r="D7" s="6">
         <v>8.6</v>
       </c>
+      <c r="G7" s="16">
+        <f t="shared" si="0"/>
+        <v>8.2666666666666657</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="1"/>
+        <v>4.1333333333333329</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -4472,6 +4511,14 @@
       <c r="D8" s="6">
         <v>9.8000000000000007</v>
       </c>
+      <c r="G8" s="16">
+        <f t="shared" si="0"/>
+        <v>9.9333333333333336</v>
+      </c>
+      <c r="H8" s="16">
+        <f t="shared" si="1"/>
+        <v>4.9666666666666668</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="7" t="s">
@@ -4480,6 +4527,13 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="7" t="s">
@@ -4489,13 +4543,21 @@
         <v>7.4</v>
       </c>
       <c r="C10" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="0"/>
+        <v>2.4666666666666668</v>
+      </c>
+      <c r="H10" s="16">
+        <f t="shared" si="1"/>
+        <v>1.2333333333333334</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
@@ -4509,10 +4571,18 @@
         <v>10</v>
       </c>
       <c r="D11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>37</v>
+      </c>
+      <c r="G11" s="16">
+        <f t="shared" si="0"/>
+        <v>6.5666666666666664</v>
+      </c>
+      <c r="H11" s="16">
+        <f t="shared" si="1"/>
+        <v>3.2833333333333328</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
@@ -4528,6 +4598,14 @@
       <c r="D12" s="6">
         <v>9.6</v>
       </c>
+      <c r="G12" s="16">
+        <f t="shared" si="0"/>
+        <v>9.4666666666666668</v>
+      </c>
+      <c r="H12" s="16">
+        <f t="shared" si="1"/>
+        <v>4.7333333333333334</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="7" t="s">
@@ -4542,13 +4620,23 @@
       <c r="D13" s="6">
         <v>6.4</v>
       </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="16">
+        <f t="shared" si="0"/>
+        <v>7.7333333333333343</v>
+      </c>
+      <c r="H13" s="16">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="9">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="C14" s="6">
         <v>10</v>
@@ -4557,6 +4645,14 @@
         <v>10</v>
       </c>
       <c r="E14" s="10"/>
+      <c r="G14" s="16">
+        <f t="shared" si="0"/>
+        <v>9.8333333333333339</v>
+      </c>
+      <c r="H14" s="16">
+        <f t="shared" si="1"/>
+        <v>4.916666666666667</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="15">
       <c r="A15" s="7" t="s">
@@ -4571,6 +4667,14 @@
       <c r="D15" s="6">
         <v>10</v>
       </c>
+      <c r="G15" s="16">
+        <f t="shared" si="0"/>
+        <v>8.9333333333333336</v>
+      </c>
+      <c r="H15" s="16">
+        <f t="shared" si="1"/>
+        <v>4.4666666666666668</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="15">
       <c r="A16" s="7" t="s">
@@ -4585,8 +4689,16 @@
       <c r="D16" s="6">
         <v>8.6999999999999993</v>
       </c>
+      <c r="G16" s="16">
+        <f t="shared" si="0"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="H16" s="16">
+        <f t="shared" si="1"/>
+        <v>4.333333333333333</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
@@ -4599,8 +4711,16 @@
       <c r="D17" s="6">
         <v>10</v>
       </c>
+      <c r="G17" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H17" s="16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="18" spans="1:5" ht="17.25" customHeight="1">
+    <row r="18" spans="1:8" ht="17.25" customHeight="1">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
@@ -4611,13 +4731,21 @@
         <v>8</v>
       </c>
       <c r="D18" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
         <v>37</v>
       </c>
+      <c r="G18" s="16">
+        <f t="shared" si="0"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="H18" s="16">
+        <f t="shared" si="1"/>
+        <v>2.8333333333333335</v>
+      </c>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
@@ -4630,8 +4758,16 @@
       <c r="D19" s="6">
         <v>10</v>
       </c>
+      <c r="G19" s="16">
+        <f t="shared" si="0"/>
+        <v>9.2666666666666675</v>
+      </c>
+      <c r="H19" s="16">
+        <f t="shared" si="1"/>
+        <v>4.6333333333333337</v>
+      </c>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="7" t="s">
         <v>17</v>
       </c>
@@ -4642,13 +4778,21 @@
         <v>10</v>
       </c>
       <c r="D20" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
         <v>37</v>
       </c>
+      <c r="G20" s="16">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="H20" s="16">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
+      </c>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
@@ -4661,8 +4805,16 @@
       <c r="D21" s="6">
         <v>9</v>
       </c>
+      <c r="G21" s="16">
+        <f t="shared" si="0"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="H21" s="16">
+        <f t="shared" si="1"/>
+        <v>4.333333333333333</v>
+      </c>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="7" t="s">
         <v>19</v>
       </c>
@@ -4675,8 +4827,15 @@
       <c r="D22" s="6">
         <v>9.5</v>
       </c>
+      <c r="G22" s="16">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="H22" s="16">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="7" t="s">
         <v>20</v>
       </c>
@@ -4689,21 +4848,36 @@
       <c r="D23" s="6">
         <v>10</v>
       </c>
+      <c r="G23" s="16">
+        <f t="shared" si="0"/>
+        <v>9.8333333333333339</v>
+      </c>
+      <c r="H23" s="16">
+        <f t="shared" si="1"/>
+        <v>4.916666666666667</v>
+      </c>
     </row>
-    <row r="24" spans="1:5" ht="15">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
+      <c r="G24" s="16">
+        <v>0</v>
+      </c>
+      <c r="H24" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:5" ht="15">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" s="6">
         <v>9</v>
@@ -4711,8 +4885,16 @@
       <c r="D25" s="6">
         <v>10</v>
       </c>
+      <c r="G25" s="16">
+        <f t="shared" si="0"/>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="H25" s="16">
+        <f t="shared" si="1"/>
+        <v>4.666666666666667</v>
+      </c>
     </row>
-    <row r="26" spans="1:5" ht="15">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="7" t="s">
         <v>23</v>
       </c>
@@ -4725,16 +4907,31 @@
       <c r="D26" s="6">
         <v>9.9</v>
       </c>
+      <c r="G26" s="16">
+        <f t="shared" si="0"/>
+        <v>9.8666666666666671</v>
+      </c>
+      <c r="H26" s="16">
+        <f t="shared" si="1"/>
+        <v>4.9333333333333336</v>
+      </c>
     </row>
-    <row r="27" spans="1:5" ht="15">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
+      <c r="G27" s="16">
+        <v>0</v>
+      </c>
+      <c r="H27" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1">
+    <row r="28" spans="1:8" ht="18" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
@@ -4747,8 +4944,16 @@
       <c r="D28" s="6">
         <v>10</v>
       </c>
+      <c r="G28" s="16">
+        <f t="shared" si="0"/>
+        <v>9.8666666666666671</v>
+      </c>
+      <c r="H28" s="16">
+        <f t="shared" si="1"/>
+        <v>4.9333333333333336</v>
+      </c>
     </row>
-    <row r="29" spans="1:5" ht="15">
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="7" t="s">
         <v>26</v>
       </c>
@@ -4761,16 +4966,31 @@
       <c r="D29" s="6">
         <v>10</v>
       </c>
+      <c r="G29" s="16">
+        <f t="shared" si="0"/>
+        <v>9.2666666666666675</v>
+      </c>
+      <c r="H29" s="16">
+        <f t="shared" si="1"/>
+        <v>4.6333333333333337</v>
+      </c>
     </row>
-    <row r="30" spans="1:5" ht="15">
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
+      <c r="G30" s="16">
+        <v>0</v>
+      </c>
+      <c r="H30" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:5" ht="15">
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="7" t="s">
         <v>28</v>
       </c>
@@ -4783,8 +5003,16 @@
       <c r="D31" s="6">
         <v>9</v>
       </c>
+      <c r="G31" s="16">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="H31" s="16">
+        <f t="shared" si="1"/>
+        <v>4.833333333333333</v>
+      </c>
     </row>
-    <row r="32" spans="1:5" ht="15">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="7" t="s">
         <v>29</v>
       </c>
@@ -4797,8 +5025,16 @@
       <c r="D32" s="6">
         <v>9</v>
       </c>
+      <c r="G32" s="16">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="H32" s="16">
+        <f t="shared" si="1"/>
+        <v>4.833333333333333</v>
+      </c>
     </row>
-    <row r="33" spans="1:4" ht="15">
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="7" t="s">
         <v>30</v>
       </c>
@@ -4811,14 +5047,29 @@
       <c r="D33" s="6">
         <v>7</v>
       </c>
+      <c r="G33" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H33" s="16">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="34" spans="1:4" ht="15">
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
+      <c r="G34" s="16">
+        <v>0</v>
+      </c>
+      <c r="H34" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>